<commit_message>
added .env with recipe api key
</commit_message>
<xml_diff>
--- a/Schema.xlsx
+++ b/Schema.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dhint\dev\my-projects\Whats_Cookin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dhint\dev\my-projects\whats_cookin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{392848F4-636A-48E1-9B37-F437E7F6FEE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2697C00F-6C06-49FB-9AA5-17A43B848E84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{E227A949-707C-4F48-9E43-2C3CC10BF1F6}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="76">
   <si>
     <t>User</t>
   </si>
@@ -283,12 +283,24 @@
   <si>
     <t>4. Bake at 350 for 20 mins</t>
   </si>
+  <si>
+    <t>return 5 recipes based on keyword</t>
+  </si>
+  <si>
+    <t>https://api.spoonacular.com/recipes/search?query=KEYWORD&amp;number=5&amp;instructionsRequired=true&amp;apiKey=ENV["RecipeAPI_KEY"]</t>
+  </si>
+  <si>
+    <t>https://api.spoonacular.com/recipes/RECIPE_ID/information?apiKey=ENV["RecipeAPI_KEY"]</t>
+  </si>
+  <si>
+    <t>returns info such as ingredients (w/ amounts) &amp; instructions</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -407,6 +419,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -634,10 +654,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -645,16 +666,71 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -682,69 +758,16 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1825,10 +1848,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0D9BCE8-7769-4713-89F9-969AB42B8643}">
-  <dimension ref="A1:AC27"/>
+  <dimension ref="A1:AC31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1846,38 +1869,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="F1" s="7" t="s">
+      <c r="B1" s="42"/>
+      <c r="F1" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="8"/>
-      <c r="I1" s="7" t="s">
+      <c r="G1" s="42"/>
+      <c r="I1" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="8"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="23" t="s">
+      <c r="J1" s="42"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="23"/>
-      <c r="S1" s="24"/>
+      <c r="O1" s="43"/>
+      <c r="P1" s="43"/>
+      <c r="Q1" s="43"/>
+      <c r="R1" s="43"/>
+      <c r="S1" s="12"/>
       <c r="T1" t="s">
         <v>43</v>
       </c>
-      <c r="X1" s="22"/>
-      <c r="Y1" s="47" t="s">
+      <c r="X1" s="11"/>
+      <c r="Y1" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="Z1" s="48"/>
-      <c r="AA1" s="48"/>
-      <c r="AB1" s="48"/>
-      <c r="AC1" s="24"/>
+      <c r="Z1" s="30"/>
+      <c r="AA1" s="30"/>
+      <c r="AB1" s="30"/>
+      <c r="AC1" s="12"/>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -1899,17 +1922,17 @@
         <v>11</v>
       </c>
       <c r="M2" s="1"/>
-      <c r="N2" s="25"/>
-      <c r="O2" s="25"/>
-      <c r="P2" s="25"/>
-      <c r="Q2" s="25"/>
-      <c r="R2" s="25"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="13"/>
       <c r="S2" s="2"/>
       <c r="X2" s="1"/>
-      <c r="Y2" s="25"/>
-      <c r="Z2" s="25"/>
-      <c r="AA2" s="25"/>
-      <c r="AB2" s="25"/>
+      <c r="Y2" s="13"/>
+      <c r="Z2" s="13"/>
+      <c r="AA2" s="13"/>
+      <c r="AB2" s="13"/>
       <c r="AC2" s="2"/>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.3">
@@ -1932,13 +1955,13 @@
         <v>25</v>
       </c>
       <c r="M3" s="1"/>
-      <c r="N3" s="13" t="s">
+      <c r="N3" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="O3" s="14"/>
-      <c r="P3" s="14"/>
-      <c r="Q3" s="14"/>
-      <c r="R3" s="15"/>
+      <c r="O3" s="45"/>
+      <c r="P3" s="45"/>
+      <c r="Q3" s="45"/>
+      <c r="R3" s="46"/>
       <c r="S3" s="2"/>
       <c r="T3" t="s">
         <v>44</v>
@@ -1949,14 +1972,14 @@
       <c r="X3" s="1">
         <v>1</v>
       </c>
-      <c r="Y3" s="49" t="s">
+      <c r="Y3" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="Z3" s="25"/>
-      <c r="AA3" s="43" t="s">
+      <c r="Z3" s="13"/>
+      <c r="AA3" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="AB3" s="44"/>
+      <c r="AB3" s="38"/>
       <c r="AC3" s="2"/>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.3">
@@ -1972,7 +1995,7 @@
       <c r="G4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="8" t="s">
         <v>22</v>
       </c>
       <c r="I4" s="1" t="s">
@@ -1982,21 +2005,21 @@
         <v>11</v>
       </c>
       <c r="M4" s="1"/>
-      <c r="N4" s="16"/>
-      <c r="O4" s="17"/>
-      <c r="P4" s="17"/>
-      <c r="Q4" s="17"/>
-      <c r="R4" s="18"/>
+      <c r="N4" s="47"/>
+      <c r="O4" s="48"/>
+      <c r="P4" s="48"/>
+      <c r="Q4" s="48"/>
+      <c r="R4" s="49"/>
       <c r="S4" s="2"/>
       <c r="X4" s="1"/>
-      <c r="Y4" s="25" t="s">
+      <c r="Y4" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="Z4" s="25" t="s">
+      <c r="Z4" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="AA4" s="45"/>
-      <c r="AB4" s="46"/>
+      <c r="AA4" s="39"/>
+      <c r="AB4" s="40"/>
       <c r="AC4" s="2"/>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.3">
@@ -2006,7 +2029,7 @@
       <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="7" t="s">
         <v>12</v>
       </c>
       <c r="F5" s="1" t="s">
@@ -2022,17 +2045,17 @@
         <v>24</v>
       </c>
       <c r="M5" s="1"/>
-      <c r="N5" s="19"/>
-      <c r="O5" s="20"/>
-      <c r="P5" s="20"/>
-      <c r="Q5" s="20"/>
-      <c r="R5" s="21"/>
+      <c r="N5" s="50"/>
+      <c r="O5" s="51"/>
+      <c r="P5" s="51"/>
+      <c r="Q5" s="51"/>
+      <c r="R5" s="52"/>
       <c r="S5" s="2"/>
       <c r="X5" s="1"/>
-      <c r="Y5" s="25"/>
-      <c r="Z5" s="25"/>
-      <c r="AA5" s="25"/>
-      <c r="AB5" s="25"/>
+      <c r="Y5" s="13"/>
+      <c r="Z5" s="13"/>
+      <c r="AA5" s="13"/>
+      <c r="AB5" s="13"/>
       <c r="AC5" s="2"/>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.3">
@@ -2042,13 +2065,13 @@
       <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="9" t="s">
         <v>23</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="8" t="s">
         <v>22</v>
       </c>
       <c r="F6" s="1"/>
@@ -2056,23 +2079,23 @@
       <c r="I6" s="1"/>
       <c r="J6" s="2"/>
       <c r="M6" s="1"/>
-      <c r="N6" s="25"/>
-      <c r="O6" s="25"/>
-      <c r="P6" s="25"/>
-      <c r="Q6" s="25"/>
-      <c r="R6" s="25"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="13"/>
+      <c r="R6" s="13"/>
       <c r="S6" s="2"/>
       <c r="X6" s="1">
         <v>2</v>
       </c>
-      <c r="Y6" s="50" t="s">
+      <c r="Y6" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="Z6" s="25"/>
-      <c r="AA6" s="43" t="s">
+      <c r="Z6" s="13"/>
+      <c r="AA6" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="AB6" s="44"/>
+      <c r="AB6" s="38"/>
       <c r="AC6" s="2"/>
     </row>
     <row r="7" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2090,26 +2113,26 @@
       <c r="I7" s="3"/>
       <c r="J7" s="4"/>
       <c r="M7" s="1"/>
-      <c r="N7" s="32" t="s">
+      <c r="N7" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="O7" s="25"/>
-      <c r="P7" s="25"/>
-      <c r="Q7" s="25"/>
-      <c r="R7" s="25"/>
+      <c r="O7" s="13"/>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="13"/>
+      <c r="R7" s="13"/>
       <c r="S7" s="2"/>
       <c r="T7" t="s">
         <v>45</v>
       </c>
       <c r="X7" s="1"/>
-      <c r="Y7" s="25" t="s">
+      <c r="Y7" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="Z7" s="25" t="s">
+      <c r="Z7" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="AA7" s="45"/>
-      <c r="AB7" s="46"/>
+      <c r="AA7" s="39"/>
+      <c r="AB7" s="40"/>
       <c r="AC7" s="2"/>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.3">
@@ -2124,22 +2147,22 @@
       </c>
       <c r="G8" s="2"/>
       <c r="M8" s="1"/>
-      <c r="N8" s="26" t="s">
+      <c r="N8" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="O8" s="25"/>
-      <c r="P8" s="25"/>
-      <c r="Q8" s="25"/>
-      <c r="R8" s="25"/>
+      <c r="O8" s="13"/>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="13"/>
+      <c r="R8" s="13"/>
       <c r="S8" s="2"/>
       <c r="T8" t="s">
         <v>46</v>
       </c>
       <c r="X8" s="1"/>
-      <c r="Y8" s="25"/>
-      <c r="Z8" s="25"/>
-      <c r="AA8" s="25"/>
-      <c r="AB8" s="25"/>
+      <c r="Y8" s="13"/>
+      <c r="Z8" s="13"/>
+      <c r="AA8" s="13"/>
+      <c r="AB8" s="13"/>
       <c r="AC8" s="2"/>
     </row>
     <row r="9" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2148,19 +2171,19 @@
       <c r="F9" s="3"/>
       <c r="G9" s="4"/>
       <c r="M9" s="1"/>
-      <c r="N9" s="27" t="s">
+      <c r="N9" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="O9" s="25">
+      <c r="O9" s="13">
         <v>1</v>
       </c>
-      <c r="P9" s="25" t="s">
+      <c r="P9" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="Q9" s="25" t="s">
+      <c r="Q9" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="R9" s="25"/>
+      <c r="R9" s="13"/>
       <c r="S9" s="2"/>
       <c r="T9" t="s">
         <v>47</v>
@@ -2168,14 +2191,14 @@
       <c r="X9" s="1">
         <v>3</v>
       </c>
-      <c r="Y9" s="50" t="s">
+      <c r="Y9" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="Z9" s="25"/>
-      <c r="AA9" s="43" t="s">
+      <c r="Z9" s="13"/>
+      <c r="AA9" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="AB9" s="44"/>
+      <c r="AB9" s="38"/>
       <c r="AC9" s="2"/>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.3">
@@ -2184,275 +2207,292 @@
       </c>
       <c r="B10" s="2"/>
       <c r="M10" s="1"/>
-      <c r="N10" s="27" t="s">
+      <c r="N10" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="O10" s="25">
+      <c r="O10" s="13">
         <v>5</v>
       </c>
-      <c r="P10" s="25" t="s">
+      <c r="P10" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="Q10" s="25" t="s">
+      <c r="Q10" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="R10" s="25"/>
+      <c r="R10" s="13"/>
       <c r="S10" s="2"/>
       <c r="T10" t="s">
         <v>52</v>
       </c>
       <c r="X10" s="1"/>
-      <c r="Y10" s="25" t="s">
+      <c r="Y10" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="Z10" s="25" t="s">
+      <c r="Z10" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="AA10" s="45"/>
-      <c r="AB10" s="46"/>
+      <c r="AA10" s="39"/>
+      <c r="AB10" s="40"/>
       <c r="AC10" s="2"/>
     </row>
     <row r="11" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3"/>
       <c r="B11" s="4"/>
       <c r="M11" s="1"/>
-      <c r="N11" s="27" t="s">
+      <c r="N11" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="O11" s="25">
+      <c r="O11" s="13">
         <v>2</v>
       </c>
-      <c r="P11" s="25" t="s">
+      <c r="P11" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="Q11" s="25" t="s">
+      <c r="Q11" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="R11" s="25"/>
+      <c r="R11" s="13"/>
       <c r="S11" s="2"/>
       <c r="T11" t="s">
         <v>53</v>
       </c>
       <c r="X11" s="1"/>
-      <c r="Y11" s="25"/>
-      <c r="Z11" s="25"/>
-      <c r="AA11" s="25"/>
-      <c r="AB11" s="25"/>
+      <c r="Y11" s="13"/>
+      <c r="Z11" s="13"/>
+      <c r="AA11" s="13"/>
+      <c r="AB11" s="13"/>
       <c r="AC11" s="2"/>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.3">
       <c r="M12" s="1"/>
-      <c r="N12" s="25"/>
-      <c r="O12" s="25"/>
-      <c r="P12" s="25"/>
-      <c r="Q12" s="25"/>
-      <c r="R12" s="25"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="13"/>
+      <c r="P12" s="13"/>
+      <c r="Q12" s="13"/>
+      <c r="R12" s="13"/>
       <c r="S12" s="2"/>
       <c r="X12" s="1"/>
-      <c r="Y12" s="25"/>
-      <c r="Z12" s="25"/>
-      <c r="AA12" s="25"/>
-      <c r="AB12" s="25"/>
+      <c r="Y12" s="13"/>
+      <c r="Z12" s="13"/>
+      <c r="AA12" s="13"/>
+      <c r="AB12" s="13"/>
       <c r="AC12" s="2"/>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.3">
       <c r="M13" s="1"/>
-      <c r="N13" s="25"/>
-      <c r="O13" s="25"/>
-      <c r="P13" s="25"/>
-      <c r="Q13" s="25"/>
-      <c r="R13" s="25"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="13"/>
+      <c r="P13" s="13"/>
+      <c r="Q13" s="13"/>
+      <c r="R13" s="13"/>
       <c r="S13" s="2"/>
       <c r="X13" s="1"/>
-      <c r="Y13" s="25"/>
-      <c r="Z13" s="25"/>
-      <c r="AA13" s="25"/>
-      <c r="AB13" s="25"/>
+      <c r="Y13" s="13"/>
+      <c r="Z13" s="13"/>
+      <c r="AA13" s="13"/>
+      <c r="AB13" s="13"/>
       <c r="AC13" s="2"/>
     </row>
     <row r="14" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="M14" s="1"/>
-      <c r="N14" s="32" t="s">
+      <c r="N14" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="O14" s="25"/>
-      <c r="P14" s="25"/>
-      <c r="Q14" s="25"/>
-      <c r="R14" s="25"/>
+      <c r="O14" s="13"/>
+      <c r="P14" s="13"/>
+      <c r="Q14" s="13"/>
+      <c r="R14" s="13"/>
       <c r="S14" s="2"/>
       <c r="T14" t="s">
         <v>45</v>
       </c>
       <c r="X14" s="3"/>
-      <c r="Y14" s="31"/>
-      <c r="Z14" s="31"/>
-      <c r="AA14" s="31"/>
-      <c r="AB14" s="31"/>
+      <c r="Y14" s="17"/>
+      <c r="Z14" s="17"/>
+      <c r="AA14" s="17"/>
+      <c r="AB14" s="17"/>
       <c r="AC14" s="4"/>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.3">
       <c r="M15" s="1"/>
-      <c r="N15" s="28" t="s">
+      <c r="N15" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="O15" s="25"/>
-      <c r="P15" s="25"/>
-      <c r="Q15" s="25"/>
-      <c r="R15" s="25"/>
+      <c r="O15" s="13"/>
+      <c r="P15" s="13"/>
+      <c r="Q15" s="13"/>
+      <c r="R15" s="13"/>
       <c r="S15" s="2"/>
       <c r="T15" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="L16" s="34" t="s">
+      <c r="L16" s="20" t="s">
         <v>54</v>
       </c>
       <c r="M16" s="1"/>
-      <c r="N16" s="27" t="s">
+      <c r="N16" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="O16" s="25" t="s">
+      <c r="O16" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="P16" s="25"/>
-      <c r="Q16" s="25"/>
-      <c r="R16" s="25"/>
+      <c r="P16" s="13"/>
+      <c r="Q16" s="13"/>
+      <c r="R16" s="13"/>
       <c r="S16" s="2"/>
       <c r="T16" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="17" spans="12:20" x14ac:dyDescent="0.3">
-      <c r="L17" s="34" t="s">
+      <c r="Y16" s="55" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="12:25" x14ac:dyDescent="0.3">
+      <c r="L17" s="20" t="s">
         <v>54</v>
       </c>
       <c r="M17" s="1"/>
-      <c r="N17" s="27" t="s">
+      <c r="N17" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="O17" s="25" t="s">
+      <c r="O17" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="P17" s="25"/>
-      <c r="Q17" s="25"/>
-      <c r="R17" s="25"/>
+      <c r="P17" s="13"/>
+      <c r="Q17" s="13"/>
+      <c r="R17" s="13"/>
       <c r="S17" s="2"/>
       <c r="T17" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="18" spans="12:20" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="L18" s="34" t="s">
+      <c r="Y17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="12:25" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L18" s="20" t="s">
         <v>55</v>
       </c>
       <c r="M18" s="1"/>
-      <c r="N18" s="27" t="s">
+      <c r="N18" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="O18" s="29" t="s">
+      <c r="O18" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="P18" s="29"/>
-      <c r="Q18" s="29"/>
-      <c r="R18" s="29"/>
-      <c r="S18" s="30"/>
-      <c r="T18" s="33" t="s">
+      <c r="P18" s="53"/>
+      <c r="Q18" s="53"/>
+      <c r="R18" s="53"/>
+      <c r="S18" s="54"/>
+      <c r="T18" s="19" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="12:20" x14ac:dyDescent="0.3">
-      <c r="L19" s="34" t="s">
+    <row r="19" spans="12:25" x14ac:dyDescent="0.3">
+      <c r="L19" s="20" t="s">
         <v>55</v>
       </c>
       <c r="M19" s="1"/>
-      <c r="N19" s="27" t="s">
+      <c r="N19" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="O19" s="25" t="s">
+      <c r="O19" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="P19" s="25"/>
-      <c r="Q19" s="25"/>
-      <c r="R19" s="25"/>
+      <c r="P19" s="13"/>
+      <c r="Q19" s="13"/>
+      <c r="R19" s="13"/>
       <c r="S19" s="2"/>
       <c r="T19" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="12:20" x14ac:dyDescent="0.3">
+    <row r="20" spans="12:25" x14ac:dyDescent="0.3">
       <c r="M20" s="1"/>
-      <c r="N20" s="25"/>
-      <c r="O20" s="25"/>
-      <c r="P20" s="25"/>
-      <c r="Q20" s="25"/>
-      <c r="R20" s="25"/>
+      <c r="N20" s="13"/>
+      <c r="O20" s="13"/>
+      <c r="P20" s="13"/>
+      <c r="Q20" s="13"/>
+      <c r="R20" s="13"/>
       <c r="S20" s="2"/>
     </row>
-    <row r="21" spans="12:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="12:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="M21" s="3"/>
-      <c r="N21" s="31"/>
-      <c r="O21" s="31"/>
-      <c r="P21" s="31"/>
-      <c r="Q21" s="31"/>
-      <c r="R21" s="31"/>
+      <c r="N21" s="17"/>
+      <c r="O21" s="17"/>
+      <c r="P21" s="17"/>
+      <c r="Q21" s="17"/>
+      <c r="R21" s="17"/>
       <c r="S21" s="4"/>
     </row>
-    <row r="23" spans="12:20" x14ac:dyDescent="0.3">
-      <c r="L23" s="51"/>
-      <c r="M23" s="51"/>
-      <c r="N23" s="51"/>
-      <c r="O23" s="51"/>
-      <c r="P23" s="52" t="s">
+    <row r="23" spans="12:25" x14ac:dyDescent="0.3">
+      <c r="L23" s="33"/>
+      <c r="M23" s="33"/>
+      <c r="N23" s="33"/>
+      <c r="O23" s="33"/>
+      <c r="P23" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="Q23" s="53" t="s">
+      <c r="Q23" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="R23" s="51" t="s">
+      <c r="R23" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="S23" s="51"/>
-      <c r="T23" s="51"/>
-    </row>
-    <row r="24" spans="12:20" x14ac:dyDescent="0.3">
-      <c r="P24" s="54" t="s">
+      <c r="S23" s="33"/>
+      <c r="T23" s="33"/>
+    </row>
+    <row r="24" spans="12:25" x14ac:dyDescent="0.3">
+      <c r="P24" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="Q24" s="35"/>
-      <c r="R24" s="36"/>
-    </row>
-    <row r="25" spans="12:20" x14ac:dyDescent="0.3">
-      <c r="M25" s="12" t="s">
+      <c r="Q24" s="21"/>
+      <c r="R24" s="22"/>
+    </row>
+    <row r="25" spans="12:25" x14ac:dyDescent="0.3">
+      <c r="M25" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="P25" s="37" t="s">
+      <c r="P25" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="Q25" s="38" t="s">
+      <c r="Q25" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="R25" s="39"/>
-    </row>
-    <row r="26" spans="12:20" x14ac:dyDescent="0.3">
-      <c r="M26" s="12" t="s">
+      <c r="R25" s="25"/>
+    </row>
+    <row r="26" spans="12:25" x14ac:dyDescent="0.3">
+      <c r="M26" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="P26" s="37" t="s">
+      <c r="P26" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="Q26" s="38" t="s">
+      <c r="Q26" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="R26" s="39"/>
-    </row>
-    <row r="27" spans="12:20" x14ac:dyDescent="0.3">
-      <c r="P27" s="40"/>
-      <c r="Q27" s="41"/>
-      <c r="R27" s="42"/>
+      <c r="R26" s="25"/>
+    </row>
+    <row r="27" spans="12:25" x14ac:dyDescent="0.3">
+      <c r="P27" s="26"/>
+      <c r="Q27" s="27"/>
+      <c r="R27" s="28"/>
+    </row>
+    <row r="30" spans="12:25" x14ac:dyDescent="0.3">
+      <c r="M30" s="55" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="31" spans="12:25" x14ac:dyDescent="0.3">
+      <c r="M31" t="s">
+        <v>75</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="O18:S18"/>
     <mergeCell ref="AA3:AB4"/>
     <mergeCell ref="AA6:AB7"/>
     <mergeCell ref="AA9:AB10"/>
@@ -2461,9 +2501,12 @@
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="N1:R1"/>
     <mergeCell ref="N3:R5"/>
-    <mergeCell ref="O18:S18"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="Y16" r:id="rId1" xr:uid="{3A97F97F-A81E-48B1-B394-CD25BFF0E5F6}"/>
+    <hyperlink ref="M30" r:id="rId2" xr:uid="{49B07B4E-03A8-44E9-8106-B42A03CBF882}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>